<commit_message>
change logic variant name
</commit_message>
<xml_diff>
--- a/Template Data - Bulk Product.xlsx
+++ b/Template Data - Bulk Product.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Product Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Variant Type</t>
   </si>
   <si>
-    <t>Variant Name</t>
-  </si>
-  <si>
     <t>Variant SKU Code</t>
   </si>
   <si>
@@ -121,15 +118,15 @@
     <t>Size</t>
   </si>
   <si>
+    <t>coryBipSet:S</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958258/pawship%20catalog/products/zulnycreweusk0vobbqx.webp</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
-    <t>coryBipSet:S</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958258/pawship%20catalog/products/zulnycreweusk0vobbqx.webp</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958932/pawship%20catalog/products/size/agg9xvik7vrlqcg3duxr.webp</t>
   </si>
   <si>
@@ -142,24 +139,24 @@
     <t>https://res.cloudinary.com/do1uyohvw/video/upload/v1761958419/pawship%20catalog/products/niaaxvidmfkd5uuvnxov.mp4</t>
   </si>
   <si>
+    <t>coryBipSet:M</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958294/pawship%20catalog/products/clmv9r5kgt7av4fccwxg.webp</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
-    <t>coryBipSet:M</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958294/pawship%20catalog/products/clmv9r5kgt7av4fccwxg.webp</t>
+    <t>coryBipSet:L</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958364/pawship%20catalog/products/hene8wixg55pnsse9ch6.webp</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>coryBipSet:L</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958364/pawship%20catalog/products/hene8wixg55pnsse9ch6.webp</t>
-  </si>
-  <si>
     <t>MARIO HARNESS</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>Size, Color</t>
   </si>
   <si>
-    <t>Boy-S</t>
-  </si>
-  <si>
     <t>marioHarness:Boy:S</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1763388938/pawship%20catalog/products/vx9hapqtpwgi5dnt0x8g.jpg</t>
   </si>
   <si>
-    <t>Boy-M</t>
-  </si>
-  <si>
     <t>marioHarness:Boy:M</t>
   </si>
   <si>
@@ -208,16 +199,10 @@
     <t>M, Boy</t>
   </si>
   <si>
-    <t>Girl-M</t>
-  </si>
-  <si>
     <t>marioHarness:Girl:M</t>
   </si>
   <si>
     <t>M, Girl</t>
-  </si>
-  <si>
-    <t>Girl-L</t>
   </si>
   <si>
     <t>marioHarness:Girl:L</t>
@@ -233,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -268,6 +253,10 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -327,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -363,6 +352,9 @@
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -592,14 +584,13 @@
     <col customWidth="1" min="6" max="6" width="17.63"/>
     <col customWidth="1" min="7" max="7" width="15.38"/>
     <col customWidth="1" min="8" max="9" width="19.38"/>
-    <col customWidth="1" min="10" max="10" width="17.63"/>
-    <col customWidth="1" min="11" max="11" width="20.5"/>
-    <col customWidth="1" min="12" max="13" width="16.38"/>
-    <col customWidth="1" min="19" max="20" width="22.0"/>
-    <col customWidth="1" min="21" max="25" width="23.88"/>
-    <col customWidth="1" min="26" max="26" width="25.88"/>
-    <col customWidth="1" min="27" max="27" width="23.5"/>
-    <col customWidth="1" min="28" max="28" width="24.25"/>
+    <col customWidth="1" min="10" max="10" width="20.5"/>
+    <col customWidth="1" min="11" max="12" width="16.38"/>
+    <col customWidth="1" min="18" max="19" width="22.0"/>
+    <col customWidth="1" min="20" max="24" width="23.88"/>
+    <col customWidth="1" min="25" max="25" width="25.88"/>
+    <col customWidth="1" min="26" max="26" width="23.5"/>
+    <col customWidth="1" min="27" max="27" width="24.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -654,7 +645,7 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -683,78 +674,72 @@
       </c>
       <c r="AA1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D2" s="4">
         <v>1.0</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>10.0</v>
       </c>
-      <c r="O2" s="6">
+      <c r="N2" s="6">
         <v>150000.0</v>
       </c>
+      <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="9" t="s">
+      <c r="R2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="9"/>
       <c r="U2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="Y2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" s="12"/>
@@ -767,26 +752,24 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>5.0</v>
       </c>
-      <c r="O3" s="6">
+      <c r="N3" s="6">
         <v>170000.0</v>
       </c>
+      <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
@@ -796,111 +779,104 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
       <c r="J4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="M4" s="1">
         <v>15.0</v>
       </c>
-      <c r="O4" s="6">
+      <c r="N4" s="6">
         <v>170000.0</v>
       </c>
+      <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D5" s="4">
         <v>5.0</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="16">
+        <v>10.0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>125000.0</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="6">
+        <v>10.4</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="S5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="15">
-        <v>10.0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>125000.0</v>
-      </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="6">
-        <v>10.4</v>
-      </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
     </row>
     <row r="6">
       <c r="A6" s="12"/>
@@ -913,26 +889,24 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="15">
+      <c r="M6" s="16">
         <v>7.0</v>
       </c>
-      <c r="O6" s="6">
+      <c r="N6" s="6">
         <v>125000.0</v>
       </c>
+      <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="12"/>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
@@ -942,7 +916,6 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
     </row>
     <row r="7">
       <c r="A7" s="12"/>
@@ -955,26 +928,24 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="15">
+        <v>62</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="16">
         <v>3.0</v>
       </c>
+      <c r="N7" s="6">
+        <v>150000.0</v>
+      </c>
       <c r="O7" s="6">
-        <v>150000.0</v>
-      </c>
-      <c r="P7" s="6">
         <v>10.5</v>
       </c>
+      <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -984,64 +955,60 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
-      <c r="AB7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N8" s="15">
+        <v>64</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="16">
         <v>2.0</v>
       </c>
-      <c r="O8" s="6">
+      <c r="N8" s="6">
         <v>170000.0</v>
       </c>
+      <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="W2:W4"/>
     <mergeCell ref="X2:X4"/>
     <mergeCell ref="Y2:Y4"/>
     <mergeCell ref="Z2:Z4"/>
     <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="AB2:AB4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="R2:R4"/>
     <mergeCell ref="S2:S4"/>
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="U2:U4"/>
     <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:W4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -1056,34 +1023,34 @@
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="F5:F8"/>
     <mergeCell ref="G5:G8"/>
+    <mergeCell ref="W5:W8"/>
     <mergeCell ref="X5:X8"/>
     <mergeCell ref="Y5:Y8"/>
     <mergeCell ref="Z5:Z8"/>
     <mergeCell ref="AA5:AA8"/>
-    <mergeCell ref="AB5:AB8"/>
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="I5:I8"/>
+    <mergeCell ref="R5:R8"/>
     <mergeCell ref="S5:S8"/>
     <mergeCell ref="T5:T8"/>
     <mergeCell ref="U5:U8"/>
     <mergeCell ref="V5:V8"/>
-    <mergeCell ref="W5:W8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H2"/>
-    <hyperlink r:id="rId2" ref="L2"/>
-    <hyperlink r:id="rId3" ref="S2"/>
-    <hyperlink r:id="rId4" ref="U2"/>
-    <hyperlink r:id="rId5" ref="V2"/>
-    <hyperlink r:id="rId6" ref="Z2"/>
-    <hyperlink r:id="rId7" ref="L3"/>
-    <hyperlink r:id="rId8" ref="L4"/>
-    <hyperlink r:id="rId9" ref="L5"/>
-    <hyperlink r:id="rId10" ref="S5"/>
-    <hyperlink r:id="rId11" ref="T5"/>
-    <hyperlink r:id="rId12" ref="U5"/>
-    <hyperlink r:id="rId13" ref="L6"/>
-    <hyperlink r:id="rId14" ref="L8"/>
+    <hyperlink r:id="rId2" ref="K2"/>
+    <hyperlink r:id="rId3" ref="R2"/>
+    <hyperlink r:id="rId4" ref="T2"/>
+    <hyperlink r:id="rId5" ref="U2"/>
+    <hyperlink r:id="rId6" ref="Y2"/>
+    <hyperlink r:id="rId7" ref="K3"/>
+    <hyperlink r:id="rId8" ref="K4"/>
+    <hyperlink r:id="rId9" ref="K5"/>
+    <hyperlink r:id="rId10" ref="R5"/>
+    <hyperlink r:id="rId11" ref="S5"/>
+    <hyperlink r:id="rId12" ref="T5"/>
+    <hyperlink r:id="rId13" ref="K6"/>
+    <hyperlink r:id="rId14" ref="K8"/>
   </hyperlinks>
   <drawing r:id="rId15"/>
 </worksheet>

</xml_diff>

<commit_message>
gdrive link, upload to cloudinary
</commit_message>
<xml_diff>
--- a/Template Data - Bulk Product.xlsx
+++ b/Template Data - Bulk Product.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Categories" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
   <si>
     <t>Product Name</t>
   </si>
@@ -100,16 +101,13 @@
     <t>BIP/Collar</t>
   </si>
   <si>
-    <t>Cory BIP  Mendapat Bip dan Topi</t>
-  </si>
-  <si>
     <t>bip,set</t>
   </si>
   <si>
-    <t>Singapora, Australia</t>
-  </si>
-  <si>
-    <t>2 Week</t>
+    <t>Singapore, Australia</t>
+  </si>
+  <si>
+    <t>2-3 Weeks</t>
   </si>
   <si>
     <t>https://pawship.id/</t>
@@ -178,7 +176,7 @@
     <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1761958703/pawship%20catalog/products/z3agvkszieyssvflgh9b.webp</t>
   </si>
   <si>
-    <t>L, Boy</t>
+    <t>L, Red</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/do1uyohvw/image/upload/v1763388934/pawship%20catalog/products/size/urrkiqyt1tqya0nroday.webp</t>
@@ -212,13 +210,199 @@
   </si>
   <si>
     <t>L, Girl</t>
+  </si>
+  <si>
+    <t>Xin BIP Couple Boy and Girl</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1MywBTdbuwiBAwTEmyLOLm1OV5hkMHJOl?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Type,Size,Color</t>
+  </si>
+  <si>
+    <t>XinBipBoy:XS</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1X2VZGzF6UVLoYRyLS0vY5KxH3qvTQpLs/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Boy,XS,Blue</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1I75v8jI3SceQR6hQSPVQIi9AOBHny_JT/view?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>XinBipBoy:S</t>
+  </si>
+  <si>
+    <t>Boy,S,Blue</t>
+  </si>
+  <si>
+    <t>XinBipBoy:M</t>
+  </si>
+  <si>
+    <t>Boy,M,Blue</t>
+  </si>
+  <si>
+    <t>XinBipBoy:L</t>
+  </si>
+  <si>
+    <t>Boy,L,Blue</t>
+  </si>
+  <si>
+    <t>XinBipBoy:XL</t>
+  </si>
+  <si>
+    <t>Boy,XL,Blue</t>
+  </si>
+  <si>
+    <t>XinBipBoy:XXL</t>
+  </si>
+  <si>
+    <t>Boy,XXL,Blue</t>
+  </si>
+  <si>
+    <t>XinBipGirl:XS</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14pnS_UiWPiLOP-5ItSkhP1J096aUWsK8/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>Girl,XS,Blue</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/18TiYpDVrscxwrbM8lGi3S4oYdarQ6C7u/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>XinBipGirl:S</t>
+  </si>
+  <si>
+    <t>Girl,S,Blue</t>
+  </si>
+  <si>
+    <t>XinBipGirl:M</t>
+  </si>
+  <si>
+    <t>Girl,M,Blue</t>
+  </si>
+  <si>
+    <t>XinBipGirl:L</t>
+  </si>
+  <si>
+    <t>Girl,L,Blue</t>
+  </si>
+  <si>
+    <t>XinBipGirl:XL</t>
+  </si>
+  <si>
+    <t>Girl,XL,Blue</t>
+  </si>
+  <si>
+    <t>XinBipGirl:XXL</t>
+  </si>
+  <si>
+    <t>Girl,XXL,Blue</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch </t>
+  </si>
+  <si>
+    <t>BIP</t>
+  </si>
+  <si>
+    <t>Chinese New Year</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costume </t>
+  </si>
+  <si>
+    <t>Hua</t>
+  </si>
+  <si>
+    <t>Dress</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ling (boy &amp; Girl) </t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xin (boy girl blue red) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christmas </t>
+  </si>
+  <si>
+    <t>Happiness</t>
+  </si>
+  <si>
+    <t>Essentials</t>
+  </si>
+  <si>
+    <t>Prosperity</t>
+  </si>
+  <si>
+    <t>T-shirt</t>
+  </si>
+  <si>
+    <t>Best Selling</t>
+  </si>
+  <si>
+    <t>Hongbao</t>
+  </si>
+  <si>
+    <t>Scarf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring </t>
+  </si>
+  <si>
+    <t>Wealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuxedo </t>
+  </si>
+  <si>
+    <t>Blossom</t>
+  </si>
+  <si>
+    <t>Costumes</t>
+  </si>
+  <si>
+    <t>T-Shirt</t>
+  </si>
+  <si>
+    <t>Shirts</t>
+  </si>
+  <si>
+    <t>Formal</t>
+  </si>
+  <si>
+    <t>Casual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -256,6 +440,24 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -360,6 +562,24 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -369,6 +589,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -576,10 +800,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.88"/>
+    <col customWidth="1" min="1" max="1" width="24.5"/>
     <col customWidth="1" min="2" max="2" width="15.5"/>
-    <col customWidth="1" min="3" max="3" width="26.75"/>
-    <col customWidth="1" min="4" max="4" width="16.0"/>
+    <col customWidth="1" min="3" max="3" width="86.38"/>
+    <col customWidth="1" min="4" max="4" width="15.25"/>
     <col customWidth="1" min="5" max="5" width="18.88"/>
     <col customWidth="1" min="6" max="6" width="17.63"/>
     <col customWidth="1" min="7" max="7" width="15.38"/>
@@ -683,35 +907,84 @@
       <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
+      <c r="C2" s="3" t="str">
+        <f>"Give your pawfriend the perfect blend of comfort and style with our ethically handmade " &amp;A2&amp;" . Designed with love to celebrate the friendship between Pawrents and their Pawfriends, it's made to fit beautifully and feel great all day long.
+Material: [Cotton / Twill / Linen / Knit / etc.]
+Texture: Soft, lightweight, breathable
+Care: Hand wash or "&amp;"gentle cycle. Air dry for best shape retention.
+Stretch: Yes/No
+Opening: Velcro/button/Zipper/none
+Measurement: 
+Measure using a soft ribbon or string around the neck or chest depending on the clothing type.
+Allow extra ± 2 cm to ensure comfort for fur a"&amp;"nd movement.
+Use our sizing chart to choose the right size for your pawfriend.
+If your pet needs extra adjustments or falls between sizes:
+👉 We offer custom sizing! Chat with our agent to customize fit (additional charges may apply).
+OR to be safe, take "&amp;"the bigger size!
+Shipping Info: 
+Items are shipped within 1–3 days.
+Pre-order items require 1-3 weeks (depending on workload &amp; production).
+Shipping fees will be confirmed during final order checkout/WhatsApp confirmation.
+Why You’ll Love It:
+Ethically "&amp;"handmade with premium finishing
+Designed for all breeds
+Comfortable for everyday wear
+Perfect for walks, photoshoots, &amp; special occasions
+Good to Know:
+Custom color requests may be available for selected products
+Accessories may vary slightly due to hand"&amp;"made nature"</f>
+        <v>Give your pawfriend the perfect blend of comfort and style with our ethically handmade CORY BIP SET . Designed with love to celebrate the friendship between Pawrents and their Pawfriends, it's made to fit beautifully and feel great all day long.
+Material: [Cotton / Twill / Linen / Knit / etc.]
+Texture: Soft, lightweight, breathable
+Care: Hand wash or gentle cycle. Air dry for best shape retention.
+Stretch: Yes/No
+Opening: Velcro/button/Zipper/none
+Measurement: 
+Measure using a soft ribbon or string around the neck or chest depending on the clothing type.
+Allow extra ± 2 cm to ensure comfort for fur and movement.
+Use our sizing chart to choose the right size for your pawfriend.
+If your pet needs extra adjustments or falls between sizes:
+👉 We offer custom sizing! Chat with our agent to customize fit (additional charges may apply).
+OR to be safe, take the bigger size!
+Shipping Info: 
+Items are shipped within 1–3 days.
+Pre-order items require 1-3 weeks (depending on workload &amp; production).
+Shipping fees will be confirmed during final order checkout/WhatsApp confirmation.
+Why You’ll Love It:
+Ethically handmade with premium finishing
+Designed for all breeds
+Comfortable for everyday wear
+Perfect for walks, photoshoots, &amp; special occasions
+Good to Know:
+Custom color requests may be available for selected products
+Accessories may vary slightly due to handmade nature</v>
       </c>
       <c r="D2" s="4">
         <v>1.0</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="M2" s="1">
         <v>10.0</v>
@@ -723,20 +996,20 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
       <c r="Y2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
@@ -752,13 +1025,13 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="M3" s="1">
         <v>5.0</v>
@@ -780,7 +1053,7 @@
       <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
     </row>
-    <row r="4">
+    <row r="4" ht="381.75" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -791,13 +1064,13 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="L4" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="M4" s="1">
         <v>15.0</v>
@@ -821,34 +1094,34 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D5" s="4">
         <v>5.0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="M5" s="16">
         <v>10.0</v>
@@ -862,13 +1135,13 @@
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="U5" s="15"/>
       <c r="V5" s="15"/>
@@ -889,13 +1162,13 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="L6" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="M6" s="16">
         <v>7.0</v>
@@ -928,11 +1201,11 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M7" s="16">
         <v>3.0</v>
@@ -967,13 +1240,13 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="L8" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="M8" s="16">
         <v>2.0</v>
@@ -995,8 +1268,333 @@
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
     </row>
+    <row r="9" ht="130.5" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>"Give your pawfriend the perfect blend of comfort and style with our ethically handmade " &amp;A9&amp;" . Designed with love to celebrate the friendship between Pawrents and their Pawfriends, it's made to fit beautifully and feel great all day long.
+Material: [Cotton / Twill / Linen / Knit / etc.]
+Texture: Soft, lightweight, breathable
+Care: Hand wash or "&amp;"gentle cycle. Air dry for best shape retention.
+Stretch: Yes/No
+Opening: Velcro/button/Zipper/none
+Measurement: 
+Measure using a soft ribbon or string around the neck or chest depending on the clothing type.
+Allow extra ± 2 cm to ensure comfort for fur a"&amp;"nd movement.
+Use our sizing chart to choose the right size for your pawfriend.
+If your pet needs extra adjustments or falls between sizes:
+👉 We offer custom sizing! Chat with our agent to customize fit (additional charges may apply).
+OR to be safe, take "&amp;"the bigger size!
+Shipping Info: 
+Items are shipped within 1–3 days.
+Pre-order items require 1-3 weeks (depending on workload &amp; production).
+Shipping fees will be confirmed during final order checkout/WhatsApp confirmation.
+Why You’ll Love It:
+Ethically "&amp;"handmade with premium finishing
+Designed for all breeds
+Comfortable for everyday wear
+Perfect for walks, photoshoots, &amp; special occasions
+Good to Know:
+Custom color requests may be available for selected products
+Accessories may vary slightly due to hand"&amp;"made nature"</f>
+        <v>Give your pawfriend the perfect blend of comfort and style with our ethically handmade Xin BIP Couple Boy and Girl . Designed with love to celebrate the friendship between Pawrents and their Pawfriends, it's made to fit beautifully and feel great all day long.
+Material: [Cotton / Twill / Linen / Knit / etc.]
+Texture: Soft, lightweight, breathable
+Care: Hand wash or gentle cycle. Air dry for best shape retention.
+Stretch: Yes/No
+Opening: Velcro/button/Zipper/none
+Measurement: 
+Measure using a soft ribbon or string around the neck or chest depending on the clothing type.
+Allow extra ± 2 cm to ensure comfort for fur and movement.
+Use our sizing chart to choose the right size for your pawfriend.
+If your pet needs extra adjustments or falls between sizes:
+👉 We offer custom sizing! Chat with our agent to customize fit (additional charges may apply).
+OR to be safe, take the bigger size!
+Shipping Info: 
+Items are shipped within 1–3 days.
+Pre-order items require 1-3 weeks (depending on workload &amp; production).
+Shipping fees will be confirmed during final order checkout/WhatsApp confirmation.
+Why You’ll Love It:
+Ethically handmade with premium finishing
+Designed for all breeds
+Comfortable for everyday wear
+Perfect for walks, photoshoots, &amp; special occasions
+Good to Know:
+Custom color requests may be available for selected products
+Accessories may vary slightly due to handmade nature</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="N9" s="19">
+        <v>185000.0</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" ht="130.5" customHeight="1">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="11" ht="130.5" customHeight="1">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="N14" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="19">
+        <v>185000.0</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="N17" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="N19" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" s="19">
+        <v>185000.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="49">
     <mergeCell ref="W2:W4"/>
     <mergeCell ref="X2:X4"/>
     <mergeCell ref="Y2:Y4"/>
@@ -1016,6 +1614,20 @@
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
+    <mergeCell ref="W5:W8"/>
+    <mergeCell ref="X5:X8"/>
+    <mergeCell ref="Y5:Y8"/>
+    <mergeCell ref="Z5:Z8"/>
+    <mergeCell ref="AA5:AA8"/>
+    <mergeCell ref="R9:R14"/>
+    <mergeCell ref="R15:R20"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="R5:R8"/>
+    <mergeCell ref="S5:S8"/>
+    <mergeCell ref="T5:T8"/>
+    <mergeCell ref="U5:U8"/>
+    <mergeCell ref="V5:V8"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
@@ -1023,18 +1635,15 @@
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="F5:F8"/>
     <mergeCell ref="G5:G8"/>
-    <mergeCell ref="W5:W8"/>
-    <mergeCell ref="X5:X8"/>
-    <mergeCell ref="Y5:Y8"/>
-    <mergeCell ref="Z5:Z8"/>
-    <mergeCell ref="AA5:AA8"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="R5:R8"/>
-    <mergeCell ref="S5:S8"/>
-    <mergeCell ref="T5:T8"/>
-    <mergeCell ref="U5:U8"/>
-    <mergeCell ref="V5:V8"/>
+    <mergeCell ref="H9:H20"/>
+    <mergeCell ref="I9:I20"/>
+    <mergeCell ref="A9:A20"/>
+    <mergeCell ref="B9:B20"/>
+    <mergeCell ref="C9:C20"/>
+    <mergeCell ref="D9:D20"/>
+    <mergeCell ref="E9:E20"/>
+    <mergeCell ref="F9:F20"/>
+    <mergeCell ref="G9:G20"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H2"/>
@@ -1051,7 +1660,195 @@
     <hyperlink r:id="rId12" ref="T5"/>
     <hyperlink r:id="rId13" ref="K6"/>
     <hyperlink r:id="rId14" ref="K8"/>
+    <hyperlink r:id="rId15" ref="H9"/>
+    <hyperlink r:id="rId16" ref="K9"/>
+    <hyperlink r:id="rId17" ref="R9"/>
+    <hyperlink r:id="rId18" ref="K10"/>
+    <hyperlink r:id="rId19" ref="K11"/>
+    <hyperlink r:id="rId20" ref="K12"/>
+    <hyperlink r:id="rId21" ref="K13"/>
+    <hyperlink r:id="rId22" ref="K14"/>
+    <hyperlink r:id="rId23" ref="K15"/>
+    <hyperlink r:id="rId24" ref="R15"/>
+    <hyperlink r:id="rId25" ref="K16"/>
+    <hyperlink r:id="rId26" ref="K17"/>
+    <hyperlink r:id="rId27" ref="K18"/>
+    <hyperlink r:id="rId28" ref="K19"/>
+    <hyperlink r:id="rId29" ref="K20"/>
   </hyperlinks>
-  <drawing r:id="rId15"/>
+  <drawing r:id="rId30"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="14.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>